<commit_message>
submit the hall effect
</commit_message>
<xml_diff>
--- a/变温霍尔效应/data.xlsx
+++ b/变温霍尔效应/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\86136\OneDrive\Desktop\2025近物实验\Cyh\变温霍尔效应\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F2D2486-6C16-4C04-8E68-C1291130D780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E1ACBA-B3A4-49FD-9015-580D85FB4616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="9970" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>T</t>
   </si>
@@ -51,9 +51,6 @@
     <t>I4</t>
   </si>
   <si>
-    <t>i</t>
-  </si>
-  <si>
     <t>RH</t>
   </si>
   <si>
@@ -66,6 +63,14 @@
   </si>
   <si>
     <t>B/mT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V_H</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ln(V_H)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -181,6 +186,17 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ln(R_H)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -207,10 +223,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$H$2:$H$53</c:f>
+              <c:f>Sheet1!$H$2:$H$50</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="52"/>
+                <c:ptCount val="49"/>
                 <c:pt idx="0">
                   <c:v>1.2345679012345678E-2</c:v>
                 </c:pt>
@@ -363,156 +379,156 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$I$2:$I$53</c:f>
+              <c:f>Sheet1!$J$2:$J$50</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="52"/>
+                <c:ptCount val="49"/>
                 <c:pt idx="0">
-                  <c:v>3.3188116534808003</c:v>
+                  <c:v>1.4735114173247155</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.3205294785947004</c:v>
+                  <c:v>1.4752292424386155</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.3228754148866857</c:v>
+                  <c:v>1.4775751787306008</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.3313112541979888</c:v>
+                  <c:v>1.4860110180419042</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.339233321531935</c:v>
+                  <c:v>1.4939330853758499</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.3376361605890432</c:v>
+                  <c:v>1.4923359244329586</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.3378137489397144</c:v>
+                  <c:v>1.4925135127836295</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.31935444343442</c:v>
+                  <c:v>1.4740542072783351</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.3048700180350616</c:v>
+                  <c:v>1.4595697818789768</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.2826015157487456</c:v>
+                  <c:v>1.4373012795926607</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.267094397138675</c:v>
+                  <c:v>1.4217941609825901</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.2603056346313402</c:v>
+                  <c:v>1.4150053984752555</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.2358312655176142</c:v>
+                  <c:v>1.3905310293615292</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.1861460002452819</c:v>
+                  <c:v>1.3408457640891971</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.1279659495083583</c:v>
+                  <c:v>1.2826657133522734</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.0490360455763019</c:v>
+                  <c:v>1.2037358094202171</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.9078568870519819</c:v>
+                  <c:v>1.062556650895897</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.7057141413046621</c:v>
+                  <c:v>0.86041390514857741</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.5012957538143972</c:v>
+                  <c:v>-0.34400448234168762</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.38492220687683504</c:v>
+                  <c:v>-1.4603780292792499</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.5553512465303347</c:v>
+                  <c:v>-0.28994898962575016</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.1723055502271262</c:v>
+                  <c:v>0.32700531407104155</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.5780743846801908</c:v>
+                  <c:v>0.73277414852410605</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3.2192757448895275</c:v>
+                  <c:v>1.3739755087334429</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>4.0320701427375969</c:v>
+                  <c:v>2.1867699065815116</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>4.4873715252096362</c:v>
+                  <c:v>2.6420712890535518</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>4.6049951706738046</c:v>
+                  <c:v>2.7596949345177197</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>4.6610305354847137</c:v>
+                  <c:v>2.8157302993286284</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>4.7129702235910731</c:v>
+                  <c:v>2.8676699874349882</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>4.7545164861005933</c:v>
+                  <c:v>2.9092162499445084</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>4.7771467507270566</c:v>
+                  <c:v>2.9318465145709718</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>4.801065862809164</c:v>
+                  <c:v>2.9557656266530792</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>4.8234418890985333</c:v>
+                  <c:v>2.9781416529424485</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>4.8431235289557808</c:v>
+                  <c:v>2.9978232927996959</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>4.859036909945142</c:v>
+                  <c:v>3.0137366737890572</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>4.8792349624806874</c:v>
+                  <c:v>3.0339347263246026</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>4.8852232312753809</c:v>
+                  <c:v>3.0399229951192961</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>4.8893335751282461</c:v>
+                  <c:v>3.0440333389721612</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>4.8802608179250484</c:v>
+                  <c:v>3.0349605817689631</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>4.8317279024020889</c:v>
+                  <c:v>2.9864276662460041</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>4.6988654261153853</c:v>
+                  <c:v>2.8535651899593</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>4.3227741179655474</c:v>
+                  <c:v>2.477473881809463</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>3.8507856959569566</c:v>
+                  <c:v>2.0054854598008718</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>3.4016139615473717</c:v>
+                  <c:v>1.5563137253912867</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>3.0537653048046005</c:v>
+                  <c:v>1.2084650686485157</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>2.3625035832052892</c:v>
+                  <c:v>0.51720334704920434</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>1.799231484066756</c:v>
+                  <c:v>-4.6068752089328903E-2</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>1.2620058355765456</c:v>
+                  <c:v>-0.58329440057953919</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.81977983149331135</c:v>
+                  <c:v>-1.0255204046627735</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -520,7 +536,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E24B-428B-B068-3EF46B65C1C5}"/>
+              <c16:uniqueId val="{00000000-430B-4A3F-B86E-1617C0795939}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -532,11 +548,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1406506351"/>
-        <c:axId val="1406517871"/>
+        <c:axId val="1052954240"/>
+        <c:axId val="1052956160"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1406506351"/>
+        <c:axId val="1052954240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -593,12 +609,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1406517871"/>
+        <c:crossAx val="1052956160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1406517871"/>
+        <c:axId val="1052956160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -655,7 +671,589 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1406506351"/>
+        <c:crossAx val="1052954240"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>RH</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="49"/>
+                <c:pt idx="0">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>122</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>123</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>127</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>129</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>133</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>137</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>139</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>141</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>142</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>157</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>158</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>159</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>161</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>162</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>163</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>164</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>167</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>169</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>172</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$2:$G$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="49"/>
+                <c:pt idx="0">
+                  <c:v>4.364533965244866</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.3720379146919424</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.3823064770932074</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.419431279620853</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.4545813586097944</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.4474723538704577</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.4482622432859396</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.3669036334913116</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.3041074249605051</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.2093206951026856</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.1445497630331749</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.1165086887835702</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.0169826224328586</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.8222748815165879</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.6062401263823065</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.3325434439178512</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.8937598736176935</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.3641390205371247</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.70892575039494465</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.23214849921011058</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.74830173775671416</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.3868088467614537</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.0808451816745657</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.9510268562401261</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>8.9063981042654028</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>14.042259083728281</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>15.795023696682462</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>16.705371248025276</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>17.595971563981042</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>18.342417061611375</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>18.762243285939967</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>19.216429699842021</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>19.65126382306477</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>20.041864139020536</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>20.363349131121645</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>20.778830963665087</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>20.903633491311215</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>20.989731437598731</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>20.800157977883096</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>19.814770932069511</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>17.349526066350712</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>11.911137440758292</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>7.4296998420221172</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>4.7413112164296995</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>3.3483412322274884</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1.6773301737756714</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.95497630331753547</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.55805687203791476</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.35860979462875198</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6295-424A-AD96-F7B4E6E1C2DA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1052962880"/>
+        <c:axId val="1052970080"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1052962880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1052970080"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1052970080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1052962880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -751,6 +1349,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1267,27 +1905,543 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>657411</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>178548</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>477592</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>45971</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>74706</xdr:colOff>
+      <xdr:colOff>416776</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>171825</xdr:rowOff>
+      <xdr:rowOff>106072</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="图表 1">
+        <xdr:cNvPr id="3" name="图表 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88FFA8EF-D41B-243C-AAF7-272E90D7C34B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53340129-F8CB-C36F-525D-A68CCEE53D5A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1300,6 +2454,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>75128</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>19140</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>14311</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>79241</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="图表 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E42EF5EE-2BDF-7608-A8B1-96401F9DF2CC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1571,10 +2761,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J50"/>
+  <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="X13" sqref="T13:X13"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="71" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1582,7 +2772,7 @@
     <col min="7" max="7" width="8.4140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1599,22 +2789,25 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>81</v>
       </c>
@@ -1631,22 +2824,30 @@
         <v>-24.08</v>
       </c>
       <c r="F2">
-        <f>ABS(B2-C2+D2-E2)/4</f>
+        <f t="shared" ref="F2:F33" si="0">ABS(B2-C2+D2-E2)/4</f>
         <v>27.627500000000001</v>
       </c>
+      <c r="G2">
+        <f>F2*1/(15*0.422)</f>
+        <v>4.364533965244866</v>
+      </c>
       <c r="H2">
-        <f>1/A2</f>
+        <f t="shared" ref="H2:H33" si="1">1/A2</f>
         <v>1.2345679012345678E-2</v>
       </c>
       <c r="I2">
-        <f>LN(F2)</f>
+        <f t="shared" ref="I2:I33" si="2">LN(F2)</f>
         <v>3.3188116534808003</v>
       </c>
       <c r="J2">
+        <f>LN(G2)</f>
+        <v>1.4735114173247155</v>
+      </c>
+      <c r="K2">
         <v>422</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>84</v>
       </c>
@@ -1663,19 +2864,27 @@
         <v>-24.07</v>
       </c>
       <c r="F3">
-        <f>ABS(B3-C3+D3-E3)/4</f>
+        <f t="shared" si="0"/>
         <v>27.674999999999997</v>
       </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G51" si="3">F3*1/(15*0.422)</f>
+        <v>4.3720379146919424</v>
+      </c>
       <c r="H3">
-        <f>1/A3</f>
+        <f t="shared" si="1"/>
         <v>1.1904761904761904E-2</v>
       </c>
       <c r="I3">
-        <f>LN(F3)</f>
+        <f t="shared" si="2"/>
         <v>3.3205294785947004</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J3">
+        <f t="shared" ref="J3:J50" si="4">LN(G3)</f>
+        <v>1.4752292424386155</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>87</v>
       </c>
@@ -1692,19 +2901,27 @@
         <v>-24.18</v>
       </c>
       <c r="F4">
-        <f>ABS(B4-C4+D4-E4)/4</f>
+        <f t="shared" si="0"/>
         <v>27.740000000000002</v>
       </c>
+      <c r="G4">
+        <f t="shared" si="3"/>
+        <v>4.3823064770932074</v>
+      </c>
       <c r="H4">
-        <f>1/A4</f>
+        <f t="shared" si="1"/>
         <v>1.1494252873563218E-2</v>
       </c>
       <c r="I4">
-        <f>LN(F4)</f>
+        <f t="shared" si="2"/>
         <v>3.3228754148866857</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J4">
+        <f t="shared" si="4"/>
+        <v>1.4775751787306008</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>95</v>
       </c>
@@ -1721,19 +2938,27 @@
         <v>-24.22</v>
       </c>
       <c r="F5">
-        <f>ABS(B5-C5+D5-E5)/4</f>
+        <f t="shared" si="0"/>
         <v>27.975000000000001</v>
       </c>
+      <c r="G5">
+        <f t="shared" si="3"/>
+        <v>4.419431279620853</v>
+      </c>
       <c r="H5">
-        <f>1/A5</f>
+        <f t="shared" si="1"/>
         <v>1.0526315789473684E-2</v>
       </c>
       <c r="I5">
-        <f>LN(F5)</f>
+        <f t="shared" si="2"/>
         <v>3.3313112541979888</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J5">
+        <f t="shared" si="4"/>
+        <v>1.4860110180419042</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>105</v>
       </c>
@@ -1750,19 +2975,27 @@
         <v>-24.27</v>
       </c>
       <c r="F6">
-        <f>ABS(B6-C6+D6-E6)/4</f>
+        <f t="shared" si="0"/>
         <v>28.197500000000002</v>
       </c>
+      <c r="G6">
+        <f t="shared" si="3"/>
+        <v>4.4545813586097944</v>
+      </c>
       <c r="H6">
-        <f>1/A6</f>
+        <f t="shared" si="1"/>
         <v>9.5238095238095247E-3</v>
       </c>
       <c r="I6">
-        <f>LN(F6)</f>
+        <f t="shared" si="2"/>
         <v>3.339233321531935</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J6">
+        <f t="shared" si="4"/>
+        <v>1.4939330853758499</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>110</v>
       </c>
@@ -1779,19 +3012,27 @@
         <v>-24.15</v>
       </c>
       <c r="F7">
-        <f>ABS(B7-C7+D7-E7)/4</f>
+        <f t="shared" si="0"/>
         <v>28.152499999999996</v>
       </c>
+      <c r="G7">
+        <f t="shared" si="3"/>
+        <v>4.4474723538704577</v>
+      </c>
       <c r="H7">
-        <f>1/A7</f>
+        <f t="shared" si="1"/>
         <v>9.0909090909090905E-3</v>
       </c>
       <c r="I7">
-        <f>LN(F7)</f>
+        <f t="shared" si="2"/>
         <v>3.3376361605890432</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J7">
+        <f t="shared" si="4"/>
+        <v>1.4923359244329586</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>115</v>
       </c>
@@ -1808,19 +3049,27 @@
         <v>-24.05</v>
       </c>
       <c r="F8">
-        <f>ABS(B8-C8+D8-E8)/4</f>
+        <f t="shared" si="0"/>
         <v>28.157499999999999</v>
       </c>
+      <c r="G8">
+        <f t="shared" si="3"/>
+        <v>4.4482622432859396</v>
+      </c>
       <c r="H8">
-        <f>1/A8</f>
+        <f t="shared" si="1"/>
         <v>8.6956521739130436E-3</v>
       </c>
       <c r="I8">
-        <f>LN(F8)</f>
+        <f t="shared" si="2"/>
         <v>3.3378137489397144</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J8">
+        <f t="shared" si="4"/>
+        <v>1.4925135127836295</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>117</v>
       </c>
@@ -1837,19 +3086,27 @@
         <v>-23.17</v>
       </c>
       <c r="F9">
-        <f>ABS(B9-C9+D9-E9)/4</f>
+        <f t="shared" si="0"/>
         <v>27.642500000000002</v>
       </c>
+      <c r="G9">
+        <f t="shared" si="3"/>
+        <v>4.3669036334913116</v>
+      </c>
       <c r="H9">
-        <f>1/A9</f>
+        <f t="shared" si="1"/>
         <v>8.5470085470085479E-3</v>
       </c>
       <c r="I9">
-        <f>LN(F9)</f>
+        <f t="shared" si="2"/>
         <v>3.31935444343442</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J9">
+        <f t="shared" si="4"/>
+        <v>1.4740542072783351</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>119</v>
       </c>
@@ -1866,19 +3123,27 @@
         <v>-22.63</v>
       </c>
       <c r="F10">
-        <f>ABS(B10-C10+D10-E10)/4</f>
+        <f t="shared" si="0"/>
         <v>27.244999999999997</v>
       </c>
+      <c r="G10">
+        <f t="shared" si="3"/>
+        <v>4.3041074249605051</v>
+      </c>
       <c r="H10">
-        <f>1/A10</f>
+        <f t="shared" si="1"/>
         <v>8.4033613445378148E-3</v>
       </c>
       <c r="I10">
-        <f>LN(F10)</f>
+        <f t="shared" si="2"/>
         <v>3.3048700180350616</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J10">
+        <f t="shared" si="4"/>
+        <v>1.4595697818789768</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>120</v>
       </c>
@@ -1895,19 +3160,27 @@
         <v>-22.14</v>
       </c>
       <c r="F11">
-        <f>ABS(B11-C11+D11-E11)/4</f>
+        <f t="shared" si="0"/>
         <v>26.645</v>
       </c>
+      <c r="G11">
+        <f t="shared" si="3"/>
+        <v>4.2093206951026856</v>
+      </c>
       <c r="H11">
-        <f>1/A11</f>
+        <f t="shared" si="1"/>
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="I11">
-        <f>LN(F11)</f>
+        <f t="shared" si="2"/>
         <v>3.2826015157487456</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J11">
+        <f t="shared" si="4"/>
+        <v>1.4373012795926607</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>121</v>
       </c>
@@ -1924,19 +3197,27 @@
         <v>-21.82</v>
       </c>
       <c r="F12">
-        <f>ABS(B12-C12+D12-E12)/4</f>
+        <f t="shared" si="0"/>
         <v>26.234999999999999</v>
       </c>
+      <c r="G12">
+        <f t="shared" si="3"/>
+        <v>4.1445497630331749</v>
+      </c>
       <c r="H12">
-        <f>1/A12</f>
+        <f t="shared" si="1"/>
         <v>8.2644628099173556E-3</v>
       </c>
       <c r="I12">
-        <f>LN(F12)</f>
+        <f t="shared" si="2"/>
         <v>3.267094397138675</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J12">
+        <f t="shared" si="4"/>
+        <v>1.4217941609825901</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>122</v>
       </c>
@@ -1953,19 +3234,27 @@
         <v>-21.47</v>
       </c>
       <c r="F13">
-        <f>ABS(B13-C13+D13-E13)/4</f>
+        <f t="shared" si="0"/>
         <v>26.057499999999997</v>
       </c>
+      <c r="G13">
+        <f t="shared" si="3"/>
+        <v>4.1165086887835702</v>
+      </c>
       <c r="H13">
-        <f>1/A13</f>
+        <f t="shared" si="1"/>
         <v>8.1967213114754103E-3</v>
       </c>
       <c r="I13">
-        <f>LN(F13)</f>
+        <f t="shared" si="2"/>
         <v>3.2603056346313402</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J13">
+        <f t="shared" si="4"/>
+        <v>1.4150053984752555</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>123</v>
       </c>
@@ -1982,19 +3271,27 @@
         <v>-20.82</v>
       </c>
       <c r="F14">
-        <f>ABS(B14-C14+D14-E14)/4</f>
+        <f t="shared" si="0"/>
         <v>25.427499999999995</v>
       </c>
+      <c r="G14">
+        <f t="shared" si="3"/>
+        <v>4.0169826224328586</v>
+      </c>
       <c r="H14">
-        <f>1/A14</f>
+        <f t="shared" si="1"/>
         <v>8.130081300813009E-3</v>
       </c>
       <c r="I14">
-        <f>LN(F14)</f>
+        <f t="shared" si="2"/>
         <v>3.2358312655176142</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J14">
+        <f t="shared" si="4"/>
+        <v>1.3905310293615292</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>125</v>
       </c>
@@ -2011,19 +3308,27 @@
         <v>-19.62</v>
       </c>
       <c r="F15">
-        <f>ABS(B15-C15+D15-E15)/4</f>
+        <f t="shared" si="0"/>
         <v>24.195</v>
       </c>
+      <c r="G15">
+        <f t="shared" si="3"/>
+        <v>3.8222748815165879</v>
+      </c>
       <c r="H15">
-        <f>1/A15</f>
+        <f t="shared" si="1"/>
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="I15">
-        <f>LN(F15)</f>
+        <f t="shared" si="2"/>
         <v>3.1861460002452819</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J15">
+        <f t="shared" si="4"/>
+        <v>1.3408457640891971</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>127</v>
       </c>
@@ -2040,19 +3345,27 @@
         <v>-18.170000000000002</v>
       </c>
       <c r="F16">
-        <f>ABS(B16-C16+D16-E16)/4</f>
+        <f t="shared" si="0"/>
         <v>22.827500000000001</v>
       </c>
+      <c r="G16">
+        <f t="shared" si="3"/>
+        <v>3.6062401263823065</v>
+      </c>
       <c r="H16">
-        <f>1/A16</f>
+        <f t="shared" si="1"/>
         <v>7.874015748031496E-3</v>
       </c>
       <c r="I16">
-        <f>LN(F16)</f>
+        <f t="shared" si="2"/>
         <v>3.1279659495083583</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J16">
+        <f t="shared" si="4"/>
+        <v>1.2826657133522734</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>129</v>
       </c>
@@ -2069,19 +3382,27 @@
         <v>-16.579999999999998</v>
       </c>
       <c r="F17">
-        <f>ABS(B17-C17+D17-E17)/4</f>
+        <f t="shared" si="0"/>
         <v>21.094999999999999</v>
       </c>
+      <c r="G17">
+        <f t="shared" si="3"/>
+        <v>3.3325434439178512</v>
+      </c>
       <c r="H17">
-        <f>1/A17</f>
+        <f t="shared" si="1"/>
         <v>7.7519379844961239E-3</v>
       </c>
       <c r="I17">
-        <f>LN(F17)</f>
+        <f t="shared" si="2"/>
         <v>3.0490360455763019</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J17">
+        <f t="shared" si="4"/>
+        <v>1.2037358094202171</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>131</v>
       </c>
@@ -2098,19 +3419,27 @@
         <v>-13.59</v>
       </c>
       <c r="F18">
-        <f>ABS(B18-C18+D18-E18)/4</f>
+        <f t="shared" si="0"/>
         <v>18.317499999999999</v>
       </c>
+      <c r="G18">
+        <f t="shared" si="3"/>
+        <v>2.8937598736176935</v>
+      </c>
       <c r="H18">
-        <f>1/A18</f>
+        <f t="shared" si="1"/>
         <v>7.6335877862595417E-3</v>
       </c>
       <c r="I18">
-        <f>LN(F18)</f>
+        <f t="shared" si="2"/>
         <v>2.9078568870519819</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J18">
+        <f t="shared" si="4"/>
+        <v>1.062556650895897</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>133</v>
       </c>
@@ -2127,19 +3456,27 @@
         <v>-10.46</v>
       </c>
       <c r="F19">
-        <f>ABS(B19-C19+D19-E19)/4</f>
+        <f t="shared" si="0"/>
         <v>14.965</v>
       </c>
+      <c r="G19">
+        <f t="shared" si="3"/>
+        <v>2.3641390205371247</v>
+      </c>
       <c r="H19">
-        <f>1/A19</f>
+        <f t="shared" si="1"/>
         <v>7.5187969924812026E-3</v>
       </c>
       <c r="I19">
-        <f>LN(F19)</f>
+        <f t="shared" si="2"/>
         <v>2.7057141413046621</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J19">
+        <f t="shared" si="4"/>
+        <v>0.86041390514857741</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>137</v>
       </c>
@@ -2156,19 +3493,27 @@
         <v>-0.22700000000000001</v>
       </c>
       <c r="F20">
-        <f>ABS(B20-C20+D20-E20)/4</f>
+        <f t="shared" si="0"/>
         <v>4.4874999999999998</v>
       </c>
+      <c r="G20">
+        <f t="shared" si="3"/>
+        <v>0.70892575039494465</v>
+      </c>
       <c r="H20">
-        <f>1/A20</f>
+        <f t="shared" si="1"/>
         <v>7.2992700729927005E-3</v>
       </c>
       <c r="I20">
-        <f>LN(F20)</f>
+        <f t="shared" si="2"/>
         <v>1.5012957538143972</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J20">
+        <f t="shared" si="4"/>
+        <v>-0.34400448234168762</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>139</v>
       </c>
@@ -2185,19 +3530,27 @@
         <v>6.0129999999999999</v>
       </c>
       <c r="F21">
-        <f>ABS(B21-C21+D21-E21)/4</f>
+        <f t="shared" si="0"/>
         <v>1.4695</v>
       </c>
+      <c r="G21">
+        <f t="shared" si="3"/>
+        <v>0.23214849921011058</v>
+      </c>
       <c r="H21">
-        <f>1/A21</f>
+        <f t="shared" si="1"/>
         <v>7.1942446043165471E-3</v>
       </c>
       <c r="I21">
-        <f>LN(F21)</f>
+        <f t="shared" si="2"/>
         <v>0.38492220687683504</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J21">
+        <f t="shared" si="4"/>
+        <v>-1.4603780292792499</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>140</v>
       </c>
@@ -2214,19 +3567,27 @@
         <v>9.4710000000000001</v>
       </c>
       <c r="F22">
-        <f>ABS(B22-C22+D22-E22)/4</f>
+        <f t="shared" si="0"/>
         <v>4.7367500000000007</v>
       </c>
+      <c r="G22">
+        <f t="shared" si="3"/>
+        <v>0.74830173775671416</v>
+      </c>
       <c r="H22">
-        <f>1/A22</f>
+        <f t="shared" si="1"/>
         <v>7.1428571428571426E-3</v>
       </c>
       <c r="I22">
-        <f>LN(F22)</f>
+        <f t="shared" si="2"/>
         <v>1.5553512465303347</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J22">
+        <f t="shared" si="4"/>
+        <v>-0.28994898962575016</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>141</v>
       </c>
@@ -2243,19 +3604,27 @@
         <v>13.134</v>
       </c>
       <c r="F23">
-        <f>ABS(B23-C23+D23-E23)/4</f>
+        <f t="shared" si="0"/>
         <v>8.7785000000000011</v>
       </c>
+      <c r="G23">
+        <f t="shared" si="3"/>
+        <v>1.3868088467614537</v>
+      </c>
       <c r="H23">
-        <f>1/A23</f>
+        <f t="shared" si="1"/>
         <v>7.0921985815602835E-3</v>
       </c>
       <c r="I23">
-        <f>LN(F23)</f>
+        <f t="shared" si="2"/>
         <v>2.1723055502271262</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J23">
+        <f t="shared" si="4"/>
+        <v>0.32700531407104155</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>142</v>
       </c>
@@ -2272,19 +3641,27 @@
         <v>16.978000000000002</v>
       </c>
       <c r="F24">
-        <f>ABS(B24-C24+D24-E24)/4</f>
+        <f t="shared" si="0"/>
         <v>13.171750000000001</v>
       </c>
+      <c r="G24">
+        <f t="shared" si="3"/>
+        <v>2.0808451816745657</v>
+      </c>
       <c r="H24">
-        <f>1/A24</f>
+        <f t="shared" si="1"/>
         <v>7.0422535211267607E-3</v>
       </c>
       <c r="I24">
-        <f>LN(F24)</f>
+        <f t="shared" si="2"/>
         <v>2.5780743846801908</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J24">
+        <f t="shared" si="4"/>
+        <v>0.73277414852410605</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>145</v>
       </c>
@@ -2301,19 +3678,27 @@
         <v>29.66</v>
       </c>
       <c r="F25">
-        <f>ABS(B25-C25+D25-E25)/4</f>
+        <f t="shared" si="0"/>
         <v>25.009999999999998</v>
       </c>
+      <c r="G25">
+        <f t="shared" si="3"/>
+        <v>3.9510268562401261</v>
+      </c>
       <c r="H25">
-        <f>1/A25</f>
+        <f t="shared" si="1"/>
         <v>6.8965517241379309E-3</v>
       </c>
       <c r="I25">
-        <f>LN(F25)</f>
+        <f t="shared" si="2"/>
         <v>3.2192757448895275</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J25">
+        <f t="shared" si="4"/>
+        <v>1.3739755087334429</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>150</v>
       </c>
@@ -2330,19 +3715,27 @@
         <v>58.48</v>
       </c>
       <c r="F26">
-        <f>ABS(B26-C26+D26-E26)/4</f>
+        <f t="shared" si="0"/>
         <v>56.377499999999998</v>
       </c>
+      <c r="G26">
+        <f t="shared" si="3"/>
+        <v>8.9063981042654028</v>
+      </c>
       <c r="H26">
-        <f>1/A26</f>
+        <f t="shared" si="1"/>
         <v>6.6666666666666671E-3</v>
       </c>
       <c r="I26">
-        <f>LN(F26)</f>
+        <f t="shared" si="2"/>
         <v>4.0320701427375969</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J26">
+        <f t="shared" si="4"/>
+        <v>2.1867699065815116</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>155</v>
       </c>
@@ -2359,19 +3752,27 @@
         <v>90.49</v>
       </c>
       <c r="F27">
-        <f>ABS(B27-C27+D27-E27)/4</f>
+        <f t="shared" si="0"/>
         <v>88.887500000000017</v>
       </c>
+      <c r="G27">
+        <f t="shared" si="3"/>
+        <v>14.042259083728281</v>
+      </c>
       <c r="H27">
-        <f>1/A27</f>
+        <f t="shared" si="1"/>
         <v>6.4516129032258064E-3</v>
       </c>
       <c r="I27">
-        <f>LN(F27)</f>
+        <f t="shared" si="2"/>
         <v>4.4873715252096362</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J27">
+        <f t="shared" si="4"/>
+        <v>2.6420712890535518</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>157</v>
       </c>
@@ -2388,19 +3789,27 @@
         <v>101.28</v>
       </c>
       <c r="F28">
-        <f>ABS(B28-C28+D28-E28)/4</f>
+        <f t="shared" si="0"/>
         <v>99.982499999999987</v>
       </c>
+      <c r="G28">
+        <f t="shared" si="3"/>
+        <v>15.795023696682462</v>
+      </c>
       <c r="H28">
-        <f>1/A28</f>
+        <f t="shared" si="1"/>
         <v>6.369426751592357E-3</v>
       </c>
       <c r="I28">
-        <f>LN(F28)</f>
+        <f t="shared" si="2"/>
         <v>4.6049951706738046</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J28">
+        <f t="shared" si="4"/>
+        <v>2.7596949345177197</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>158</v>
       </c>
@@ -2417,19 +3826,27 @@
         <v>107.25</v>
       </c>
       <c r="F29">
-        <f>ABS(B29-C29+D29-E29)/4</f>
+        <f t="shared" si="0"/>
         <v>105.745</v>
       </c>
+      <c r="G29">
+        <f t="shared" si="3"/>
+        <v>16.705371248025276</v>
+      </c>
       <c r="H29">
-        <f>1/A29</f>
+        <f t="shared" si="1"/>
         <v>6.3291139240506328E-3</v>
       </c>
       <c r="I29">
-        <f>LN(F29)</f>
+        <f t="shared" si="2"/>
         <v>4.6610305354847137</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J29">
+        <f t="shared" si="4"/>
+        <v>2.8157302993286284</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>159</v>
       </c>
@@ -2446,19 +3863,27 @@
         <v>111.52</v>
       </c>
       <c r="F30">
-        <f>ABS(B30-C30+D30-E30)/4</f>
+        <f t="shared" si="0"/>
         <v>111.38249999999999</v>
       </c>
+      <c r="G30">
+        <f t="shared" si="3"/>
+        <v>17.595971563981042</v>
+      </c>
       <c r="H30">
-        <f>1/A30</f>
+        <f t="shared" si="1"/>
         <v>6.2893081761006293E-3</v>
       </c>
       <c r="I30">
-        <f>LN(F30)</f>
+        <f t="shared" si="2"/>
         <v>4.7129702235910731</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J30">
+        <f t="shared" si="4"/>
+        <v>2.8676699874349882</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>160</v>
       </c>
@@ -2475,19 +3900,27 @@
         <v>116.31</v>
       </c>
       <c r="F31">
-        <f>ABS(B31-C31+D31-E31)/4</f>
+        <f t="shared" si="0"/>
         <v>116.1075</v>
       </c>
+      <c r="G31">
+        <f t="shared" si="3"/>
+        <v>18.342417061611375</v>
+      </c>
       <c r="H31">
-        <f>1/A31</f>
+        <f t="shared" si="1"/>
         <v>6.2500000000000003E-3</v>
       </c>
       <c r="I31">
-        <f>LN(F31)</f>
+        <f t="shared" si="2"/>
         <v>4.7545164861005933</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J31">
+        <f t="shared" si="4"/>
+        <v>2.9092162499445084</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>161</v>
       </c>
@@ -2504,19 +3937,27 @@
         <v>118.64</v>
       </c>
       <c r="F32">
-        <f>ABS(B32-C32+D32-E32)/4</f>
+        <f t="shared" si="0"/>
         <v>118.76499999999999</v>
       </c>
+      <c r="G32">
+        <f t="shared" si="3"/>
+        <v>18.762243285939967</v>
+      </c>
       <c r="H32">
-        <f>1/A32</f>
+        <f t="shared" si="1"/>
         <v>6.2111801242236021E-3</v>
       </c>
       <c r="I32">
-        <f>LN(F32)</f>
+        <f t="shared" si="2"/>
         <v>4.7771467507270566</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J32">
+        <f t="shared" si="4"/>
+        <v>2.9318465145709718</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>162</v>
       </c>
@@ -2533,19 +3974,27 @@
         <v>121.58</v>
       </c>
       <c r="F33">
-        <f>ABS(B33-C33+D33-E33)/4</f>
+        <f t="shared" si="0"/>
         <v>121.64</v>
       </c>
+      <c r="G33">
+        <f t="shared" si="3"/>
+        <v>19.216429699842021</v>
+      </c>
       <c r="H33">
-        <f>1/A33</f>
+        <f t="shared" si="1"/>
         <v>6.1728395061728392E-3</v>
       </c>
       <c r="I33">
-        <f>LN(F33)</f>
+        <f t="shared" si="2"/>
         <v>4.801065862809164</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J33">
+        <f t="shared" si="4"/>
+        <v>2.9557656266530792</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>163</v>
       </c>
@@ -2562,19 +4011,27 @@
         <v>124.24</v>
       </c>
       <c r="F34">
-        <f>ABS(B34-C34+D34-E34)/4</f>
+        <f t="shared" ref="F34:F51" si="5">ABS(B34-C34+D34-E34)/4</f>
         <v>124.3925</v>
       </c>
+      <c r="G34">
+        <f t="shared" si="3"/>
+        <v>19.65126382306477</v>
+      </c>
       <c r="H34">
-        <f>1/A34</f>
+        <f t="shared" ref="H34:H50" si="6">1/A34</f>
         <v>6.1349693251533744E-3</v>
       </c>
       <c r="I34">
-        <f>LN(F34)</f>
+        <f t="shared" ref="I34:I50" si="7">LN(F34)</f>
         <v>4.8234418890985333</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J34">
+        <f t="shared" si="4"/>
+        <v>2.9781416529424485</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>164</v>
       </c>
@@ -2591,19 +4048,27 @@
         <v>126.46</v>
       </c>
       <c r="F35">
-        <f>ABS(B35-C35+D35-E35)/4</f>
+        <f t="shared" si="5"/>
         <v>126.86499999999999</v>
       </c>
+      <c r="G35">
+        <f t="shared" si="3"/>
+        <v>20.041864139020536</v>
+      </c>
       <c r="H35">
-        <f>1/A35</f>
+        <f t="shared" si="6"/>
         <v>6.0975609756097563E-3</v>
       </c>
       <c r="I35">
-        <f>LN(F35)</f>
+        <f t="shared" si="7"/>
         <v>4.8431235289557808</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J35">
+        <f t="shared" si="4"/>
+        <v>2.9978232927996959</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>165</v>
       </c>
@@ -2620,19 +4085,27 @@
         <v>128.22999999999999</v>
       </c>
       <c r="F36">
-        <f>ABS(B36-C36+D36-E36)/4</f>
+        <f t="shared" si="5"/>
         <v>128.9</v>
       </c>
+      <c r="G36">
+        <f t="shared" si="3"/>
+        <v>20.363349131121645</v>
+      </c>
       <c r="H36">
-        <f>1/A36</f>
+        <f t="shared" si="6"/>
         <v>6.0606060606060606E-3</v>
       </c>
       <c r="I36">
-        <f>LN(F36)</f>
+        <f t="shared" si="7"/>
         <v>4.859036909945142</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J36">
+        <f t="shared" si="4"/>
+        <v>3.0137366737890572</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>167</v>
       </c>
@@ -2649,19 +4122,27 @@
         <v>130.63</v>
       </c>
       <c r="F37">
-        <f>ABS(B37-C37+D37-E37)/4</f>
+        <f t="shared" si="5"/>
         <v>131.53</v>
       </c>
+      <c r="G37">
+        <f t="shared" si="3"/>
+        <v>20.778830963665087</v>
+      </c>
       <c r="H37">
-        <f>1/A37</f>
+        <f t="shared" si="6"/>
         <v>5.9880239520958087E-3</v>
       </c>
       <c r="I37">
-        <f>LN(F37)</f>
+        <f t="shared" si="7"/>
         <v>4.8792349624806874</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J37">
+        <f t="shared" si="4"/>
+        <v>3.0339347263246026</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>169</v>
       </c>
@@ -2678,19 +4159,27 @@
         <v>131.22</v>
       </c>
       <c r="F38">
-        <f>ABS(B38-C38+D38-E38)/4</f>
+        <f t="shared" si="5"/>
         <v>132.32</v>
       </c>
+      <c r="G38">
+        <f t="shared" si="3"/>
+        <v>20.903633491311215</v>
+      </c>
       <c r="H38">
-        <f>1/A38</f>
+        <f t="shared" si="6"/>
         <v>5.9171597633136093E-3</v>
       </c>
       <c r="I38">
-        <f>LN(F38)</f>
+        <f t="shared" si="7"/>
         <v>4.8852232312753809</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J38">
+        <f t="shared" si="4"/>
+        <v>3.0399229951192961</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>170</v>
       </c>
@@ -2707,19 +4196,27 @@
         <v>131.79</v>
       </c>
       <c r="F39">
-        <f>ABS(B39-C39+D39-E39)/4</f>
+        <f t="shared" si="5"/>
         <v>132.86499999999998</v>
       </c>
+      <c r="G39">
+        <f t="shared" si="3"/>
+        <v>20.989731437598731</v>
+      </c>
       <c r="H39">
-        <f>1/A39</f>
+        <f t="shared" si="6"/>
         <v>5.8823529411764705E-3</v>
       </c>
       <c r="I39">
-        <f>LN(F39)</f>
+        <f t="shared" si="7"/>
         <v>4.8893335751282461</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J39">
+        <f t="shared" si="4"/>
+        <v>3.0440333389721612</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>172</v>
       </c>
@@ -2736,19 +4233,27 @@
         <v>130.11000000000001</v>
       </c>
       <c r="F40">
-        <f>ABS(B40-C40+D40-E40)/4</f>
+        <f t="shared" si="5"/>
         <v>131.66499999999999</v>
       </c>
+      <c r="G40">
+        <f t="shared" si="3"/>
+        <v>20.800157977883096</v>
+      </c>
       <c r="H40">
-        <f>1/A40</f>
+        <f t="shared" si="6"/>
         <v>5.8139534883720929E-3</v>
       </c>
       <c r="I40">
-        <f>LN(F40)</f>
+        <f t="shared" si="7"/>
         <v>4.8802608179250484</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J40">
+        <f t="shared" si="4"/>
+        <v>3.0349605817689631</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>175</v>
       </c>
@@ -2765,19 +4270,27 @@
         <v>123.9</v>
       </c>
       <c r="F41">
-        <f>ABS(B41-C41+D41-E41)/4</f>
+        <f t="shared" si="5"/>
         <v>125.42750000000001</v>
       </c>
+      <c r="G41">
+        <f t="shared" si="3"/>
+        <v>19.814770932069511</v>
+      </c>
       <c r="H41">
-        <f>1/A41</f>
+        <f t="shared" si="6"/>
         <v>5.7142857142857143E-3</v>
       </c>
       <c r="I41">
-        <f>LN(F41)</f>
+        <f t="shared" si="7"/>
         <v>4.8317279024020889</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J41">
+        <f t="shared" si="4"/>
+        <v>2.9864276662460041</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>180</v>
       </c>
@@ -2794,19 +4307,27 @@
         <v>107.98</v>
       </c>
       <c r="F42">
-        <f>ABS(B42-C42+D42-E42)/4</f>
+        <f t="shared" si="5"/>
         <v>109.82250000000001</v>
       </c>
+      <c r="G42">
+        <f t="shared" si="3"/>
+        <v>17.349526066350712</v>
+      </c>
       <c r="H42">
-        <f>1/A42</f>
+        <f t="shared" si="6"/>
         <v>5.5555555555555558E-3</v>
       </c>
       <c r="I42">
-        <f>LN(F42)</f>
+        <f t="shared" si="7"/>
         <v>4.6988654261153853</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J42">
+        <f t="shared" si="4"/>
+        <v>2.8535651899593</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>190</v>
       </c>
@@ -2823,19 +4344,27 @@
         <v>74.13</v>
       </c>
       <c r="F43">
-        <f>ABS(B43-C43+D43-E43)/4</f>
+        <f t="shared" si="5"/>
         <v>75.397499999999994</v>
       </c>
+      <c r="G43">
+        <f t="shared" si="3"/>
+        <v>11.911137440758292</v>
+      </c>
       <c r="H43">
-        <f>1/A43</f>
+        <f t="shared" si="6"/>
         <v>5.263157894736842E-3</v>
       </c>
       <c r="I43">
-        <f>LN(F43)</f>
+        <f t="shared" si="7"/>
         <v>4.3227741179655474</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J43">
+        <f t="shared" si="4"/>
+        <v>2.477473881809463</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>200</v>
       </c>
@@ -2852,19 +4381,27 @@
         <v>46.36</v>
       </c>
       <c r="F44">
-        <f>ABS(B44-C44+D44-E44)/4</f>
+        <f t="shared" si="5"/>
         <v>47.03</v>
       </c>
+      <c r="G44">
+        <f t="shared" si="3"/>
+        <v>7.4296998420221172</v>
+      </c>
       <c r="H44">
-        <f>1/A44</f>
+        <f t="shared" si="6"/>
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="I44">
-        <f>LN(F44)</f>
+        <f t="shared" si="7"/>
         <v>3.8507856959569566</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J44">
+        <f t="shared" si="4"/>
+        <v>2.0054854598008718</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>210</v>
       </c>
@@ -2881,19 +4418,27 @@
         <v>29.67</v>
       </c>
       <c r="F45">
-        <f>ABS(B45-C45+D45-E45)/4</f>
+        <f t="shared" si="5"/>
         <v>30.012499999999999</v>
       </c>
+      <c r="G45">
+        <f t="shared" si="3"/>
+        <v>4.7413112164296995</v>
+      </c>
       <c r="H45">
-        <f>1/A45</f>
+        <f t="shared" si="6"/>
         <v>4.7619047619047623E-3</v>
       </c>
       <c r="I45">
-        <f>LN(F45)</f>
+        <f t="shared" si="7"/>
         <v>3.4016139615473717</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J45">
+        <f t="shared" si="4"/>
+        <v>1.5563137253912867</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>220</v>
       </c>
@@ -2910,19 +4455,27 @@
         <v>20.81</v>
       </c>
       <c r="F46">
-        <f>ABS(B46-C46+D46-E46)/4</f>
+        <f t="shared" si="5"/>
         <v>21.195</v>
       </c>
+      <c r="G46">
+        <f t="shared" si="3"/>
+        <v>3.3483412322274884</v>
+      </c>
       <c r="H46">
-        <f>1/A46</f>
+        <f t="shared" si="6"/>
         <v>4.5454545454545452E-3</v>
       </c>
       <c r="I46">
-        <f>LN(F46)</f>
+        <f t="shared" si="7"/>
         <v>3.0537653048046005</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J46">
+        <f t="shared" si="4"/>
+        <v>1.2084650686485157</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>240</v>
       </c>
@@ -2939,19 +4492,27 @@
         <v>10.36</v>
       </c>
       <c r="F47">
-        <f>ABS(B47-C47+D47-E47)/4</f>
+        <f t="shared" si="5"/>
         <v>10.6175</v>
       </c>
+      <c r="G47">
+        <f t="shared" si="3"/>
+        <v>1.6773301737756714</v>
+      </c>
       <c r="H47">
-        <f>1/A47</f>
+        <f t="shared" si="6"/>
         <v>4.1666666666666666E-3</v>
       </c>
       <c r="I47">
-        <f>LN(F47)</f>
+        <f t="shared" si="7"/>
         <v>2.3625035832052892</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J47">
+        <f t="shared" si="4"/>
+        <v>0.51720334704920434</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>260</v>
       </c>
@@ -2968,19 +4529,27 @@
         <v>5.87</v>
       </c>
       <c r="F48">
-        <f>ABS(B48-C48+D48-E48)/4</f>
+        <f t="shared" si="5"/>
         <v>6.0449999999999999</v>
       </c>
+      <c r="G48">
+        <f t="shared" si="3"/>
+        <v>0.95497630331753547</v>
+      </c>
       <c r="H48">
-        <f>1/A48</f>
+        <f t="shared" si="6"/>
         <v>3.8461538461538464E-3</v>
       </c>
       <c r="I48">
-        <f>LN(F48)</f>
+        <f t="shared" si="7"/>
         <v>1.799231484066756</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J48">
+        <f t="shared" si="4"/>
+        <v>-4.6068752089328903E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>280</v>
       </c>
@@ -2997,19 +4566,27 @@
         <v>3.47</v>
       </c>
       <c r="F49">
-        <f>ABS(B49-C49+D49-E49)/4</f>
+        <f t="shared" si="5"/>
         <v>3.5325000000000002</v>
       </c>
+      <c r="G49">
+        <f t="shared" si="3"/>
+        <v>0.55805687203791476</v>
+      </c>
       <c r="H49">
-        <f>1/A49</f>
+        <f t="shared" si="6"/>
         <v>3.5714285714285713E-3</v>
       </c>
       <c r="I49">
-        <f>LN(F49)</f>
+        <f t="shared" si="7"/>
         <v>1.2620058355765456</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J49">
+        <f t="shared" si="4"/>
+        <v>-0.58329440057953919</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>300</v>
       </c>
@@ -3026,16 +4603,46 @@
         <v>2.25</v>
       </c>
       <c r="F50">
-        <f>ABS(B50-C50+D50-E50)/4</f>
+        <f t="shared" si="5"/>
         <v>2.27</v>
       </c>
+      <c r="G50">
+        <f t="shared" si="3"/>
+        <v>0.35860979462875198</v>
+      </c>
       <c r="H50">
-        <f>1/A50</f>
+        <f t="shared" si="6"/>
         <v>3.3333333333333335E-3</v>
       </c>
       <c r="I50">
-        <f>LN(F50)</f>
+        <f t="shared" si="7"/>
         <v>0.81977983149331135</v>
+      </c>
+      <c r="J50">
+        <f t="shared" si="4"/>
+        <v>-1.0255204046627735</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B51">
+        <v>-2.3679999999999999</v>
+      </c>
+      <c r="C51">
+        <v>2.3679999999999999</v>
+      </c>
+      <c r="D51">
+        <v>-2.3119999999999998</v>
+      </c>
+      <c r="E51">
+        <v>2.3140000000000001</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="5"/>
+        <v>2.3405</v>
+      </c>
+      <c r="G51">
+        <f>F51*1/(15*0.422)</f>
+        <v>0.36974723538704579</v>
       </c>
     </row>
   </sheetData>

</xml_diff>